<commit_message>
Fix the bug when there was a choice with none value
I did create a function to process choices, and handle difficult case like spreadChoicesName
</commit_message>
<xml_diff>
--- a/packages/evolution-generator/src/examples/Example_Generate_Survey.xlsx
+++ b/packages/evolution-generator/src/examples/Example_Generate_Survey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Widgets"/>
@@ -528,7 +528,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,12 +546,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -603,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -643,9 +637,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1153,35 +1144,35 @@
       <c r="S4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3" t="s">
         <v>18</v>
@@ -1189,7 +1180,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
-      <c r="S5" s="14"/>
+      <c r="S5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
@@ -1649,7 +1640,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -1683,7 +1674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>52</v>
       </c>
@@ -1699,7 +1690,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -1715,7 +1706,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -1731,7 +1722,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1747,7 +1738,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -1759,7 +1750,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1775,7 +1766,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>66</v>
       </c>
@@ -1791,7 +1782,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
@@ -1807,7 +1798,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>66</v>
       </c>
@@ -1851,7 +1842,7 @@
     <col min="8" max="8" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -1943,7 +1934,7 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Add process_range function to questionnaire_dictionary
This is going to help data analyst to understand the values for input range question.
I did change the choices name to values because it's more simple to understand.
I added a first line for the first line of the csv because it's not a header for all the document.
</commit_message>
<xml_diff>
--- a/packages/evolution-generator/src/examples/Example_Generate_Survey.xlsx
+++ b/packages/evolution-generator/src/examples/Example_Generate_Survey.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Widgets"/>
@@ -1640,7 +1640,7 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
+    <sheetView workbookViewId="0">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
@@ -1826,7 +1826,7 @@
   </sheetPr>
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>

</xml_diff>